<commit_message>
SONARLINT fixed Main, service, repository, model packages and AddProductController.java; added new class ApplicationLogger.java
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport_rafael.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport_rafael.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ralph\OneDrive\Documents\Year3\Semester2\VVSS\lab01\CheckListsAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ralph\OneDrive\Documents\Year3\Semester2\VVSS\lab01\inventory\Verificare_si_validare_sisteme_soft\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_A99B5FF7B5769A7154A07A00D9F3032DEDC19295" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3356CDD-8DDA-4A13-87A3-169774161DD9}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="11_A99B5FF7B5769A7154A07A00D9F3032DEDC19295" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9DFC390C-6A8A-4F2C-8952-3A61D2696A2C}"/>
   <bookViews>
-    <workbookView xWindow="36210" yWindow="1125" windowWidth="21600" windowHeight="11385" tabRatio="650" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Main.java/line 20</t>
   </si>
   <si>
-    <t>changed System.out to System.err</t>
-  </si>
-  <si>
     <t>C09</t>
   </si>
   <si>
@@ -178,6 +175,42 @@
   </si>
   <si>
     <t>SonarLint</t>
+  </si>
+  <si>
+    <t>changed System.out to ApplicationLogger.log</t>
+  </si>
+  <si>
+    <t>Standard outputs should not be used directly to log anything</t>
+  </si>
+  <si>
+    <t>Main.java/22</t>
+  </si>
+  <si>
+    <t>System.err.println(service.getAllParts());</t>
+  </si>
+  <si>
+    <t>ApplicationLogger.log(Level.INFO, service.getAllProducts().toString());</t>
+  </si>
+  <si>
+    <t>InventoryService.java/47</t>
+  </si>
+  <si>
+    <t>Methods should not have too many parameters</t>
+  </si>
+  <si>
+    <t>public void updateInhousePart(int partIndex, int partId, String name, double price, int inStock, int min, int max, int partDynamicValue)</t>
+  </si>
+  <si>
+    <t>changing ,method requires creating new classes to wrap all the parameters into one which is too costly timewise and requires redesign of all the UML diagrams</t>
+  </si>
+  <si>
+    <t>Unused "private" fields should be removed</t>
+  </si>
+  <si>
+    <t>private int productId;</t>
+  </si>
+  <si>
+    <t>AddProductController/28</t>
   </si>
 </sst>
 </file>
@@ -392,6 +425,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -419,6 +453,9 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -434,10 +471,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,19 +835,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>31</v>
@@ -834,10 +867,10 @@
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="25"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -848,10 +881,10 @@
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="27"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -863,15 +896,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1081,19 +1114,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>31</v>
@@ -1113,10 +1146,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1127,10 +1160,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1142,15 +1175,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1349,8 +1382,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,19 +1403,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>31</v>
@@ -1395,7 +1428,7 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="18">
@@ -1406,10 +1439,10 @@
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1420,10 +1453,10 @@
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1435,15 +1468,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1473,7 +1506,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1485,10 +1518,10 @@
         <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1500,7 +1533,7 @@
         <v>39</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1509,13 +1542,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1527,7 +1560,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>35</v>
@@ -1539,13 +1572,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1716,8 +1749,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1725,9 +1758,9 @@
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="68.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="74.7109375" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.85546875" style="6"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="6"/>
@@ -1738,19 +1771,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>31</v>
@@ -1774,10 +1807,10 @@
       <c r="C4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="30"/>
+      <c r="D4" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1788,8 +1821,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1801,8 +1834,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1821,33 +1854,55 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2034,11 +2089,11 @@
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>